<commit_message>
create_quality() missing stats value
</commit_message>
<xml_diff>
--- a/data-raw/vars_label.xlsx
+++ b/data-raw/vars_label.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qc0824/Documents/2_Areas/R_Packages/canregtools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C884A27-06A7-8748-A2C1-2F64421CBBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDC8B37-386E-684A-9098-C6A8EE8C0F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{1EA01957-FAD3-6345-8E4A-0E42DDA1BA74}"/>
+    <workbookView xWindow="7880" yWindow="7160" windowWidth="34560" windowHeight="21580" activeTab="10" xr2:uid="{1EA01957-FAD3-6345-8E4A-0E42DDA1BA74}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="30" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5805" uniqueCount="4129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5805" uniqueCount="4132">
   <si>
     <t>C00</t>
   </si>
@@ -10473,6 +10473,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>国家公务员</t>
     </r>
@@ -10483,6 +10484,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>专业技术人员</t>
     </r>
@@ -10493,6 +10495,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>职员</t>
     </r>
@@ -10503,6 +10506,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>企业管理人员</t>
     </r>
@@ -10513,6 +10517,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>工人</t>
     </r>
@@ -10523,6 +10528,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>农民</t>
     </r>
@@ -10533,6 +10539,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>学生</t>
     </r>
@@ -10543,6 +10550,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>现役军人</t>
     </r>
@@ -10553,6 +10561,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>自由职业者</t>
     </r>
@@ -10563,6 +10572,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>个体经营者</t>
     </r>
@@ -10573,6 +10583,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>无业人员</t>
     </r>
@@ -10583,6 +10594,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>退（离）休人员</t>
     </r>
@@ -10593,6 +10605,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="songti"/>
+        <charset val="134"/>
       </rPr>
       <t>其他</t>
     </r>
@@ -22191,6 +22204,18 @@
   </si>
   <si>
     <t>Vars in mortality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>洛龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luolong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>淮阳区</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -22363,6 +22388,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="songti"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -25955,8 +25981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06FE49F-860C-8B46-A403-04403C7D6A51}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView topLeftCell="A203" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A195" sqref="A195:XFD195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -26933,16 +26959,16 @@
         <v>532</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>1908</v>
+        <v>1911</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>1990</v>
+        <v>1992</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>2548</v>
+        <v>4129</v>
       </c>
       <c r="E49" s="37" t="s">
-        <v>2441</v>
+        <v>4130</v>
       </c>
       <c r="F49" s="43"/>
       <c r="G49" s="43"/>
@@ -29978,16 +30004,16 @@
         <v>595</v>
       </c>
       <c r="B194" s="38" t="s">
-        <v>2241</v>
+        <v>4131</v>
       </c>
       <c r="C194" s="37" t="s">
-        <v>2110</v>
+        <v>2111</v>
       </c>
       <c r="D194" s="38" t="s">
-        <v>2587</v>
+        <v>2588</v>
       </c>
       <c r="E194" s="37" t="s">
-        <v>2481</v>
+        <v>2482</v>
       </c>
       <c r="F194" s="43"/>
       <c r="G194" s="43"/>
@@ -38260,7 +38286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483EF787-AD96-2749-AD71-91EDEE7D0A9E}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>